<commit_message>
Correção DDL e DML encaminhado
</commit_message>
<xml_diff>
--- a/Senai_HROADS_Manhã/HROADS_Fisico.xlsx
+++ b/Senai_HROADS_Manhã/HROADS_Fisico.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erika\Desktop\PROJETOS SENAI\Semestre_02\Sprint01 - Banco de Dados\senai_S02_sprint1_bd\HROADS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E9116B-5930-48F2-BB25-5F61620EF02B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{596D35E0-FFF8-4CC6-B981-C4155B8EB826}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5835" windowHeight="9765" activeTab="3" xr2:uid="{3C4F095B-4BE4-493C-BE2E-862E0EAC57D3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5835" windowHeight="9765" xr2:uid="{3C4F095B-4BE4-493C-BE2E-862E0EAC57D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Personagem" sheetId="1" r:id="rId1"/>
     <sheet name="Classe" sheetId="4" r:id="rId2"/>
-    <sheet name="Tipo Habilidade" sheetId="2" r:id="rId3"/>
+    <sheet name="ClasseHabilidade" sheetId="6" r:id="rId3"/>
     <sheet name="Habilidade" sheetId="3" r:id="rId4"/>
+    <sheet name="Tipo Habilidade" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t>BitBug</t>
   </si>
@@ -45,9 +46,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>13 = JOIN</t>
-  </si>
-  <si>
     <t>17 = WHERE</t>
   </si>
   <si>
@@ -69,9 +67,6 @@
     <t>Data Criação</t>
   </si>
   <si>
-    <t>TAREFAS 10??</t>
-  </si>
-  <si>
     <t>Ataque</t>
   </si>
   <si>
@@ -102,27 +97,6 @@
     <t>Recuperar Vida</t>
   </si>
   <si>
-    <t>T1</t>
-  </si>
-  <si>
-    <t>T2</t>
-  </si>
-  <si>
-    <t>T3</t>
-  </si>
-  <si>
-    <t>T4</t>
-  </si>
-  <si>
-    <t>H1</t>
-  </si>
-  <si>
-    <t>H2</t>
-  </si>
-  <si>
-    <t>H3</t>
-  </si>
-  <si>
     <t>C1</t>
   </si>
   <si>
@@ -144,38 +118,50 @@
     <t>Arcanista</t>
   </si>
   <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
     <t>C4</t>
   </si>
   <si>
-    <t>C5</t>
-  </si>
-  <si>
-    <t>C6</t>
-  </si>
-  <si>
     <t>C7</t>
   </si>
   <si>
     <t>Cacadora de Demonios</t>
   </si>
   <si>
-    <t>H1, H2</t>
-  </si>
-  <si>
-    <t>H3, H2</t>
+    <t>ClasseHabilidade</t>
+  </si>
+  <si>
+    <t>IDClasse</t>
+  </si>
+  <si>
+    <t>IDHabilidade</t>
+  </si>
+  <si>
+    <t>IDClasseHabilidade</t>
+  </si>
+  <si>
+    <t>10 e 13 = JOIN</t>
+  </si>
+  <si>
+    <t>TAREFAS</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>pode apagar o campo amarelo</t>
+  </si>
+  <si>
+    <t>é apenas uma anotação para quando formos resolver os exercicios</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,8 +223,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -311,8 +305,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -449,11 +473,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -481,53 +516,79 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -725,6 +786,41 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -739,14 +835,9 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -784,36 +875,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -827,10 +888,191 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1381493</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>10190</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagem 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26DD251D-007F-4EB7-926D-FDCCAAEA4ACB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2647950" y="1628775"/>
+          <a:ext cx="2638793" cy="4763165"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>657444</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>143057</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Imagem 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AC60846-29A4-41EC-9638-F12F5C8BDB9F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5934075" y="1600200"/>
+          <a:ext cx="1571844" cy="1305107"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>695551</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>47840</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Imagem 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC6B48EE-B8E8-4148-869E-2DB67CC9969C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5924550" y="3171825"/>
+          <a:ext cx="1619476" cy="1543265"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>190785</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>66956</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2021528-CCE1-4A35-8432-DB17BCABC7BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="47625" y="1581150"/>
+          <a:ext cx="2038635" cy="2010056"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{487E8D23-CBD9-47BA-B425-1239E9B61EEC}" name="Tabela2" displayName="Tabela2" ref="A2:G5" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="10" tableBorderDxfId="11" totalsRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{487E8D23-CBD9-47BA-B425-1239E9B61EEC}" name="Tabela2" displayName="Tabela2" ref="A2:G5" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{9246F545-8A9A-4240-B9DB-84AE2AFA0B64}" name="ID" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{9246F545-8A9A-4240-B9DB-84AE2AFA0B64}" name="ID" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{69C8AC8C-C5C9-45EF-B359-D23D134E0933}" name="Nome" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{2D228A13-A2E1-4BEF-87DA-80F5331E0776}" name="Classe" dataDxfId="4"/>
     <tableColumn id="4" xr3:uid="{988366CB-9734-4B2A-A372-AF5ADB70DDB0}" name="Capacidade Vida" dataDxfId="3"/>
@@ -1139,10 +1381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB5E0849-D64D-4359-96E3-E7FDFA72E572}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1154,113 +1396,121 @@
     <col min="5" max="5" width="23" customWidth="1"/>
     <col min="6" max="6" width="21.140625" customWidth="1"/>
     <col min="7" max="7" width="18.28515625" customWidth="1"/>
-    <col min="11" max="17" width="57" customWidth="1"/>
+    <col min="11" max="11" width="24" customWidth="1"/>
+    <col min="12" max="17" width="57" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:12" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="30"/>
-      <c r="K1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="35"/>
+      <c r="K1" s="31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K2" s="28"/>
+      <c r="L2" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="23">
+      <c r="C3" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="17">
         <v>100</v>
       </c>
-      <c r="E3" s="23">
+      <c r="E3" s="17">
         <v>80</v>
       </c>
-      <c r="F3" s="24">
+      <c r="F3" s="18">
         <v>44256</v>
       </c>
-      <c r="G3" s="25">
+      <c r="G3" s="19">
         <v>43483</v>
       </c>
-      <c r="K3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K3" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="23">
+      <c r="C4" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="17">
         <v>70</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="17">
         <v>100</v>
       </c>
-      <c r="F4" s="24">
+      <c r="F4" s="18">
         <v>44256</v>
       </c>
-      <c r="G4" s="25">
+      <c r="G4" s="19">
         <v>42446</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K4" s="30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" s="27">
+      <c r="C5" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="21">
         <v>75</v>
       </c>
-      <c r="E5" s="27">
+      <c r="E5" s="21">
         <v>60</v>
       </c>
-      <c r="F5" s="24">
+      <c r="F5" s="18">
         <v>44256</v>
       </c>
-      <c r="G5" s="28">
+      <c r="G5" s="22">
         <v>43177</v>
-      </c>
-      <c r="K5" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1269,116 +1519,373 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{828B9934-645A-4404-8885-DD48551A0091}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="36"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="33">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="33">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="33">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="33">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="33">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="33">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="33">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{431808FB-6473-44E0-A91F-2474F6464AC1}">
+  <dimension ref="A1:C23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="24">
+        <v>1</v>
+      </c>
+      <c r="B3" s="24">
+        <v>1</v>
+      </c>
+      <c r="C3" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="24">
+        <v>2</v>
+      </c>
+      <c r="B4" s="24">
+        <v>1</v>
+      </c>
+      <c r="C4" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="24">
+        <v>3</v>
+      </c>
+      <c r="B5" s="24">
+        <v>1</v>
+      </c>
+      <c r="C5" s="24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="27">
+        <v>4</v>
+      </c>
+      <c r="B6" s="27">
+        <v>2</v>
+      </c>
+      <c r="C6" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="27">
+        <v>5</v>
+      </c>
+      <c r="B7" s="27">
+        <v>2</v>
+      </c>
+      <c r="C7" s="27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="27">
+        <v>6</v>
+      </c>
+      <c r="B8" s="27">
+        <v>2</v>
+      </c>
+      <c r="C8" s="27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="24">
+        <v>7</v>
+      </c>
+      <c r="B9" s="24">
+        <v>3</v>
+      </c>
+      <c r="C9" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="24">
         <v>8</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="B10" s="24">
+        <v>3</v>
+      </c>
+      <c r="C10" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="24">
+        <v>9</v>
+      </c>
+      <c r="B11" s="24">
+        <v>3</v>
+      </c>
+      <c r="C11" s="24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="27">
+        <v>10</v>
+      </c>
+      <c r="B12" s="27">
         <v>4</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="C12" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="27">
+        <v>11</v>
+      </c>
+      <c r="B13" s="27">
+        <v>4</v>
+      </c>
+      <c r="C13" s="27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="27">
+        <v>12</v>
+      </c>
+      <c r="B14" s="27">
+        <v>4</v>
+      </c>
+      <c r="C14" s="27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="24">
+        <v>13</v>
+      </c>
+      <c r="B15" s="24">
+        <v>5</v>
+      </c>
+      <c r="C15" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="24">
+        <v>14</v>
+      </c>
+      <c r="B16" s="24">
+        <v>5</v>
+      </c>
+      <c r="C16" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="24">
+        <v>15</v>
+      </c>
+      <c r="B17" s="24">
+        <v>5</v>
+      </c>
+      <c r="C17" s="24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="27">
+        <v>16</v>
+      </c>
+      <c r="B18" s="27">
+        <v>6</v>
+      </c>
+      <c r="C18" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="27">
+        <v>17</v>
+      </c>
+      <c r="B19" s="27">
+        <v>6</v>
+      </c>
+      <c r="C19" s="27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="27">
+        <v>18</v>
+      </c>
+      <c r="B20" s="27">
+        <v>6</v>
+      </c>
+      <c r="C20" s="27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="24">
+        <v>19</v>
+      </c>
+      <c r="B21" s="24">
         <v>7</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C21" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="24">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="19"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="19"/>
+      <c r="B22" s="24">
+        <v>7</v>
+      </c>
+      <c r="C22" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="24">
+        <v>21</v>
+      </c>
+      <c r="B23" s="24">
+        <v>7</v>
+      </c>
+      <c r="C23" s="24">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1388,137 +1895,75 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533DE480-C243-40FF-B2D5-F73D9B87FBB7}">
-  <dimension ref="A1:B7"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A87C7E1-23CF-4810-8161-EE1290DAEF1A}">
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10:J11"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="13"/>
-    </row>
-    <row r="2" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A87C7E1-23CF-4810-8161-EE1290DAEF1A}">
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="32">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="32">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="32">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>26</v>
+      <c r="C5" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1527,4 +1972,72 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533DE480-C243-40FF-B2D5-F73D9B87FBB7}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="39"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="14">
+        <v>1</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="14">
+        <v>2</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="14">
+        <v>3</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="14">
+        <v>4</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>